<commit_message>
Show coordinates on click added.
</commit_message>
<xml_diff>
--- a/Doc/Examples/02 Onnerpolder/Dwarsraai.xlsx
+++ b/Doc/Examples/02 Onnerpolder/Dwarsraai.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/7fa01722dbc575f3/Documenten/myR_on_GitHub/shiny/mlay1D/Doc/Examples/02 Onnerpolder/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="60" documentId="13_ncr:1_{1A5750C0-1902-4B09-A746-7140F6957611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{43AD0A87-DDF8-4F8B-85A8-6379A8BD9C69}"/>
+  <xr:revisionPtr revIDLastSave="163" documentId="13_ncr:1_{1A5750C0-1902-4B09-A746-7140F6957611}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D2F2BA55-5744-4345-BCE3-9A06DE2E45F8}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{7ACBA4AB-D659-46CD-829D-BC57F2DB79A9}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{7ACBA4AB-D659-46CD-829D-BC57F2DB79A9}"/>
   </bookViews>
   <sheets>
     <sheet name="Blad1" sheetId="1" r:id="rId1"/>
@@ -521,27 +521,204 @@
         </r>
       </text>
     </comment>
+    <comment ref="B11" authorId="0" shapeId="0" xr:uid="{F1FC3AD8-CA6A-4AF5-94D5-001CBF7A1C2D}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Head on top of each section</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="C11" authorId="0" shapeId="0" xr:uid="{136BE558-D656-4BC2-ACA1-DC86E497B633}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Head on top of each section</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="D11" authorId="0" shapeId="0" xr:uid="{D5CF4029-2208-4925-BEC9-9CA3C90F2E91}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Vertical hydraulic resistance</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="E11" authorId="0" shapeId="0" xr:uid="{ABED31F7-D98D-4039-A75F-1635A1F3D4D7}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Transmissivity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="F11" authorId="0" shapeId="0" xr:uid="{5A821C5B-F7FB-48AA-926F-76020EB014C0}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nodal injections</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="G11" authorId="0" shapeId="0" xr:uid="{26BCBB28-4D09-4735-B707-A262E7D0E99B}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Vertical hydraulic resistance</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="H11" authorId="0" shapeId="0" xr:uid="{2781695A-D858-4292-A918-4171D72E7E1C}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Transmissivity</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="I11" authorId="0" shapeId="0" xr:uid="{5E85FDCA-8AE7-4046-8B73-3FB51661C47A}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Immerzeel, Kees van:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Nodal injections</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="35">
-  <si>
-    <t>Polder</t>
-  </si>
-  <si>
-    <t>Dijk</t>
-  </si>
-  <si>
-    <t>Wad</t>
-  </si>
-  <si>
-    <t>Geul</t>
-  </si>
-  <si>
-    <t>h (m+NAP)</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="47" uniqueCount="38">
   <si>
     <t>X (m)</t>
   </si>
@@ -567,9 +744,6 @@
     <t>Q2 (m2/d)</t>
   </si>
   <si>
-    <t>Aquacultuur</t>
-  </si>
-  <si>
     <t>mv</t>
   </si>
   <si>
@@ -615,9 +789,6 @@
     <t>Zonder zandbaan=1; met zandbaan=10</t>
   </si>
   <si>
-    <t xml:space="preserve">Hoofdwatergang </t>
-  </si>
-  <si>
     <t>Polder Lappenvoort</t>
   </si>
   <si>
@@ -627,10 +798,40 @@
     <t>Onnerpolder</t>
   </si>
   <si>
-    <t>Westerbroek</t>
-  </si>
-  <si>
     <t>kD boven Eem</t>
+  </si>
+  <si>
+    <t>Anisotropie</t>
+  </si>
+  <si>
+    <t>Veen/klei (Holoceen: c0, d)</t>
+  </si>
+  <si>
+    <t>Eemklei (c1, d)</t>
+  </si>
+  <si>
+    <t>kD1 (Eem, m2/d)</t>
+  </si>
+  <si>
+    <t>kD2 (Peelo, Peize, Waalre, m2/d)</t>
+  </si>
+  <si>
+    <t>Polder Westerbroek</t>
+  </si>
+  <si>
+    <t>Zomerpeil (h, m+NAP)</t>
+  </si>
+  <si>
+    <t>Stijghoogte MiPWA</t>
+  </si>
+  <si>
+    <t>Infiltratie flux MIPWA (mm/dag)</t>
+  </si>
+  <si>
+    <t>h-zomer (m+NAP)</t>
+  </si>
+  <si>
+    <t>h-winter (m+NAP)</t>
   </si>
 </sst>
 </file>
@@ -678,7 +879,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="12">
+  <fills count="11">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -693,12 +894,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="9" tint="0.59999389629810485"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -706,12 +901,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="-0.249977111117893"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.39997558519241921"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -745,6 +934,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="1">
     <border>
@@ -758,25 +953,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="18">
+  <cellXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="2" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
     <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="10" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Standaard" xfId="0" builtinId="0"/>
@@ -1096,160 +1290,201 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{61B36BD5-1B8D-46B8-962A-150B009AC3A9}">
-  <dimension ref="A1:AO37"/>
+  <dimension ref="A1:AO39"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
       <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomRight" activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.140625" customWidth="1"/>
-    <col min="2" max="2" width="7.42578125" style="1" customWidth="1"/>
-    <col min="3" max="10" width="5" style="1" customWidth="1"/>
+    <col min="1" max="1" width="34.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.28515625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="11.5703125" style="1" customWidth="1"/>
+    <col min="5" max="5" width="9.85546875" style="1" customWidth="1"/>
+    <col min="6" max="6" width="7.42578125" style="1" customWidth="1"/>
+    <col min="7" max="7" width="10.7109375" style="1" customWidth="1"/>
+    <col min="8" max="8" width="9.5703125" style="1" customWidth="1"/>
+    <col min="9" max="9" width="18.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
     <col min="11" max="11" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8" style="1" customWidth="1"/>
     <col min="13" max="14" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="15" max="15" width="8" style="1" customWidth="1"/>
     <col min="16" max="16" width="8" style="1" bestFit="1" customWidth="1"/>
     <col min="17" max="25" width="8" style="1" customWidth="1"/>
-    <col min="26" max="26" width="5" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="9.5703125" customWidth="1"/>
     <col min="27" max="33" width="5" customWidth="1"/>
     <col min="34" max="34" width="5" bestFit="1" customWidth="1"/>
     <col min="35" max="41" width="5" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="D1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="E1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="F1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="G1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="H1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="I1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="J1" s="13" t="s">
-        <v>30</v>
-      </c>
-      <c r="K1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="L1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="M1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="N1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="O1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="P1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="Q1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="R1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="S1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="T1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="U1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="V1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="W1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="X1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="Y1" s="13" t="s">
-        <v>31</v>
-      </c>
-      <c r="Z1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AA1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AB1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AC1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AD1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AE1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AF1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AG1" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="AH1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AI1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AJ1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AK1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AL1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AM1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AN1" s="13" t="s">
-        <v>33</v>
-      </c>
-      <c r="AO1" s="13" t="s">
-        <v>33</v>
+      <c r="A1" s="10" t="s">
+        <v>5</v>
+      </c>
+      <c r="B1" s="10" t="str">
+        <f>$A$12</f>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="C1" s="10" t="str">
+        <f t="shared" ref="C1:J1" si="0">$A$12</f>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="D1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="E1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="F1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="G1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="H1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="I1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="J1" s="10" t="str">
+        <f t="shared" si="0"/>
+        <v>Polder Lappenvoort</v>
+      </c>
+      <c r="K1" s="10" t="str">
+        <f>$A$13</f>
+        <v>Anisotropie</v>
+      </c>
+      <c r="L1" s="10" t="str">
+        <f t="shared" ref="L1:X1" si="1">$A$14</f>
+        <v>Hondsrug</v>
+      </c>
+      <c r="M1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="N1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="O1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="P1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="Q1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="R1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="S1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="T1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="U1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="V1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="W1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="X1" s="10" t="str">
+        <f t="shared" si="1"/>
+        <v>Hondsrug</v>
+      </c>
+      <c r="Y1" s="10" t="str">
+        <f>$A$13</f>
+        <v>Anisotropie</v>
+      </c>
+      <c r="Z1" s="10" t="str">
+        <f>$A$15</f>
+        <v>Onnerpolder</v>
+      </c>
+      <c r="AA1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AB1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AC1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AD1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AE1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AF1" s="10" t="s">
+        <v>25</v>
+      </c>
+      <c r="AG1" s="10" t="str">
+        <f>$A$16</f>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AH1" s="10" t="str">
+        <f t="shared" ref="AH1:AO1" si="2">$A$16</f>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AI1" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AJ1" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AK1" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AL1" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AM1" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AN1" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Polder Westerbroek</v>
+      </c>
+      <c r="AO1" s="10" t="str">
+        <f t="shared" si="2"/>
+        <v>Polder Westerbroek</v>
       </c>
     </row>
     <row r="2" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A2" s="6" t="s">
-        <v>5</v>
+        <v>0</v>
       </c>
       <c r="B2" s="2">
         <v>0</v>
@@ -1259,43 +1494,43 @@
         <v>200</v>
       </c>
       <c r="D2" s="2">
-        <f t="shared" ref="D2:J2" si="0">C2+200</f>
+        <f t="shared" ref="D2:J2" si="3">C2+200</f>
         <v>400</v>
       </c>
       <c r="E2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>600</v>
       </c>
       <c r="F2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>800</v>
       </c>
       <c r="G2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1000</v>
       </c>
       <c r="H2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1200</v>
       </c>
       <c r="I2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1400</v>
       </c>
       <c r="J2" s="2">
-        <f t="shared" si="0"/>
+        <f t="shared" si="3"/>
         <v>1600</v>
       </c>
-      <c r="K2" s="3">
+      <c r="K2" s="15">
         <f>J2+200</f>
         <v>1800</v>
       </c>
       <c r="L2" s="3">
-        <f t="shared" ref="L2:M2" si="1">K2+200</f>
+        <f t="shared" ref="L2:M2" si="4">K2+200</f>
         <v>2000</v>
       </c>
       <c r="M2" s="3">
-        <f t="shared" si="1"/>
+        <f t="shared" si="4"/>
         <v>2200</v>
       </c>
       <c r="N2" s="3">
@@ -1303,47 +1538,47 @@
         <v>2400</v>
       </c>
       <c r="O2" s="3">
-        <f t="shared" ref="O2:P2" si="2">N2+200</f>
+        <f t="shared" ref="O2:P2" si="5">N2+200</f>
         <v>2600</v>
       </c>
       <c r="P2" s="3">
-        <f t="shared" si="2"/>
+        <f t="shared" si="5"/>
         <v>2800</v>
       </c>
       <c r="Q2" s="3">
-        <f t="shared" ref="Q2:Y2" si="3">P2+200</f>
+        <f t="shared" ref="Q2:X2" si="6">P2+200</f>
         <v>3000</v>
       </c>
       <c r="R2" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3200</v>
       </c>
       <c r="S2" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3400</v>
       </c>
       <c r="T2" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3600</v>
       </c>
       <c r="U2" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>3800</v>
       </c>
       <c r="V2" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4000</v>
       </c>
       <c r="W2" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4200</v>
       </c>
       <c r="X2" s="3">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>4400</v>
       </c>
-      <c r="Y2" s="3">
-        <f t="shared" si="3"/>
+      <c r="Y2" s="15">
+        <f>X2+200</f>
         <v>4600</v>
       </c>
       <c r="Z2" s="4">
@@ -1351,104 +1586,104 @@
         <v>4800</v>
       </c>
       <c r="AA2" s="4">
-        <f t="shared" ref="AA2:AG2" si="4">Z2+200</f>
+        <f t="shared" ref="AA2:AG2" si="7">Z2+200</f>
         <v>5000</v>
       </c>
       <c r="AB2" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5200</v>
       </c>
       <c r="AC2" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5400</v>
       </c>
       <c r="AD2" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5600</v>
       </c>
       <c r="AE2" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>5800</v>
       </c>
       <c r="AF2" s="4">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>6000</v>
       </c>
-      <c r="AG2" s="17">
-        <f t="shared" si="4"/>
+      <c r="AG2" s="14">
+        <f t="shared" si="7"/>
         <v>6200</v>
       </c>
-      <c r="AH2" s="17">
+      <c r="AH2" s="14">
         <f>AG2+200</f>
         <v>6400</v>
       </c>
-      <c r="AI2" s="17">
-        <f t="shared" ref="AI2:AN2" si="5">AH2+200</f>
+      <c r="AI2" s="14">
+        <f t="shared" ref="AI2:AN2" si="8">AH2+200</f>
         <v>6600</v>
       </c>
-      <c r="AJ2" s="17">
-        <f t="shared" si="5"/>
+      <c r="AJ2" s="14">
+        <f t="shared" si="8"/>
         <v>6800</v>
       </c>
-      <c r="AK2" s="17">
-        <f t="shared" si="5"/>
+      <c r="AK2" s="14">
+        <f t="shared" si="8"/>
         <v>7000</v>
       </c>
-      <c r="AL2" s="17">
-        <f t="shared" si="5"/>
+      <c r="AL2" s="14">
+        <f t="shared" si="8"/>
         <v>7200</v>
       </c>
-      <c r="AM2" s="17">
-        <f t="shared" si="5"/>
+      <c r="AM2" s="14">
+        <f t="shared" si="8"/>
         <v>7400</v>
       </c>
-      <c r="AN2" s="17">
-        <f t="shared" si="5"/>
+      <c r="AN2" s="14">
+        <f t="shared" si="8"/>
         <v>7600</v>
       </c>
-      <c r="AO2" s="14"/>
+      <c r="AO2" s="11"/>
     </row>
     <row r="3" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A3" s="6" t="s">
-        <v>4</v>
+        <v>33</v>
       </c>
       <c r="B3" s="5">
-        <f t="shared" ref="B3:J3" si="6">drain_niveau</f>
+        <f t="shared" ref="B3:J3" si="9">drain_niveau</f>
         <v>-0.5</v>
       </c>
       <c r="C3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
       <c r="D3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
       <c r="E3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
       <c r="F3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
       <c r="G3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
       <c r="H3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
       <c r="I3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
       <c r="J3" s="5">
-        <f t="shared" si="6"/>
+        <f t="shared" si="9"/>
         <v>-0.5</v>
       </c>
-      <c r="K3" s="3">
+      <c r="K3" s="15">
         <v>1000</v>
       </c>
       <c r="L3" s="3">
@@ -1490,407 +1725,407 @@
       <c r="X3" s="3">
         <v>1000</v>
       </c>
-      <c r="Y3" s="3">
+      <c r="Y3" s="15">
         <v>1000</v>
       </c>
       <c r="Z3" s="4">
-        <f>drain_niveau</f>
+        <f t="shared" ref="Z3:AF3" si="10">drain_niveau</f>
         <v>-0.5</v>
       </c>
       <c r="AA3" s="4">
-        <f>drain_niveau</f>
+        <f t="shared" si="10"/>
         <v>-0.5</v>
       </c>
       <c r="AB3" s="4">
-        <f>drain_niveau</f>
+        <f t="shared" si="10"/>
         <v>-0.5</v>
       </c>
       <c r="AC3" s="4">
-        <f>drain_niveau</f>
+        <f t="shared" si="10"/>
         <v>-0.5</v>
       </c>
       <c r="AD3" s="4">
-        <f>drain_niveau</f>
+        <f t="shared" si="10"/>
         <v>-0.5</v>
       </c>
       <c r="AE3" s="4">
-        <f>drain_niveau</f>
+        <f t="shared" si="10"/>
         <v>-0.5</v>
       </c>
       <c r="AF3" s="4">
-        <f>drain_niveau</f>
+        <f t="shared" si="10"/>
         <v>-0.5</v>
       </c>
-      <c r="AG3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AG3" s="14">
+        <f t="shared" ref="AG3:AO3" si="11">drain_niveau-0.8</f>
         <v>-1.3</v>
       </c>
-      <c r="AH3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AH3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
-      <c r="AI3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AI3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
-      <c r="AJ3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AJ3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
-      <c r="AK3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AK3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
-      <c r="AL3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AL3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
-      <c r="AM3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AM3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
-      <c r="AN3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AN3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
-      <c r="AO3" s="17">
-        <f>drain_niveau-0.8</f>
+      <c r="AO3" s="14">
+        <f t="shared" si="11"/>
         <v>-1.3</v>
       </c>
     </row>
     <row r="4" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A4" s="6" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" s="16">
-        <f t="shared" ref="B4:J4" si="7">c0</f>
+        <v>28</v>
+      </c>
+      <c r="B4" s="13">
+        <f t="shared" ref="B4:J4" si="12">c0</f>
         <v>57.142857142857146</v>
       </c>
-      <c r="C4" s="16">
-        <f t="shared" si="7"/>
+      <c r="C4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="D4" s="16">
-        <f t="shared" si="7"/>
+      <c r="D4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="E4" s="16">
-        <f t="shared" si="7"/>
+      <c r="E4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="F4" s="16">
-        <f t="shared" si="7"/>
+      <c r="F4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="G4" s="16">
-        <f t="shared" si="7"/>
+      <c r="G4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="H4" s="16">
-        <f t="shared" si="7"/>
+      <c r="H4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="I4" s="16">
-        <f t="shared" si="7"/>
+      <c r="I4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="J4" s="16">
-        <f t="shared" si="7"/>
+      <c r="J4" s="13">
+        <f t="shared" si="12"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="K4" s="3">
-        <f t="shared" ref="K4:Y4" si="8">10^6</f>
+      <c r="K4" s="15">
+        <f t="shared" ref="K4:Y4" si="13">10^6</f>
         <v>1000000</v>
       </c>
       <c r="L4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="M4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="N4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="O4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="P4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="Q4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="R4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="S4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="T4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="U4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="V4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="W4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="X4" s="3">
-        <f t="shared" si="8"/>
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
-      <c r="Y4" s="3">
-        <f t="shared" si="8"/>
+      <c r="Y4" s="15">
+        <f t="shared" si="13"/>
         <v>1000000</v>
       </c>
       <c r="Z4" s="4">
-        <f>c0</f>
+        <f t="shared" ref="Z4:AO4" si="14">c0</f>
         <v>57.142857142857146</v>
       </c>
       <c r="AA4" s="4">
-        <f>c0</f>
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
       <c r="AB4" s="4">
-        <f>c0</f>
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
       <c r="AC4" s="4">
-        <f>c0</f>
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
       <c r="AD4" s="4">
-        <f>c0</f>
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
       <c r="AE4" s="4">
-        <f>c0</f>
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
       <c r="AF4" s="4">
-        <f>c0</f>
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AG4" s="17">
-        <f>c0</f>
+      <c r="AG4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AH4" s="17">
-        <f>c0</f>
+      <c r="AH4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AI4" s="17">
-        <f>c0</f>
+      <c r="AI4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AJ4" s="17">
-        <f>c0</f>
+      <c r="AJ4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AK4" s="17">
-        <f>c0</f>
+      <c r="AK4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AL4" s="17">
-        <f>c0</f>
+      <c r="AL4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AM4" s="17">
-        <f>c0</f>
+      <c r="AM4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AN4" s="17">
-        <f>c0</f>
+      <c r="AN4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
-      <c r="AO4" s="17">
-        <f>c0</f>
+      <c r="AO4" s="14">
+        <f t="shared" si="14"/>
         <v>57.142857142857146</v>
       </c>
     </row>
     <row r="5" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A5" s="6" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B5" s="2">
-        <f t="shared" ref="B5:J5" si="9">kD_zandbaan</f>
+        <f t="shared" ref="B5:J5" si="15">kD_zandbaan</f>
         <v>500</v>
       </c>
       <c r="C5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>500</v>
       </c>
       <c r="D5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>500</v>
       </c>
       <c r="E5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>500</v>
       </c>
       <c r="F5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>500</v>
       </c>
       <c r="G5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>500</v>
       </c>
       <c r="H5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>500</v>
       </c>
       <c r="I5" s="2">
-        <f t="shared" si="9"/>
+        <f t="shared" si="15"/>
         <v>500</v>
       </c>
       <c r="J5" s="2">
-        <f t="shared" si="9"/>
-        <v>500</v>
-      </c>
-      <c r="K5" s="3">
-        <f t="shared" ref="K5:AG5" si="10">kD_zandbaan</f>
+        <f t="shared" si="15"/>
+        <v>500</v>
+      </c>
+      <c r="K5" s="15">
+        <f t="shared" ref="K5:AG5" si="16">kD_zandbaan</f>
         <v>500</v>
       </c>
       <c r="L5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="M5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="N5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="O5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="P5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="Q5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="R5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="S5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="T5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="U5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="V5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="W5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="X5" s="3">
-        <f t="shared" si="10"/>
-        <v>500</v>
-      </c>
-      <c r="Y5" s="3">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="Y5" s="15">
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="Z5" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="AA5" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="AB5" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="AC5" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="AD5" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="AE5" s="4">
-        <f t="shared" si="10"/>
+        <f t="shared" si="16"/>
         <v>500</v>
       </c>
       <c r="AF5" s="4">
-        <f t="shared" si="10"/>
-        <v>500</v>
-      </c>
-      <c r="AG5" s="17">
-        <f t="shared" si="10"/>
-        <v>500</v>
-      </c>
-      <c r="AH5" s="17">
-        <f t="shared" ref="AH5:AO5" si="11">kD_zandbaan</f>
-        <v>500</v>
-      </c>
-      <c r="AI5" s="17">
-        <f t="shared" si="11"/>
-        <v>500</v>
-      </c>
-      <c r="AJ5" s="17">
-        <f t="shared" si="11"/>
-        <v>500</v>
-      </c>
-      <c r="AK5" s="17">
-        <f t="shared" si="11"/>
-        <v>500</v>
-      </c>
-      <c r="AL5" s="17">
-        <f t="shared" si="11"/>
-        <v>500</v>
-      </c>
-      <c r="AM5" s="17">
-        <f t="shared" si="11"/>
-        <v>500</v>
-      </c>
-      <c r="AN5" s="17">
-        <f t="shared" si="11"/>
-        <v>500</v>
-      </c>
-      <c r="AO5" s="17">
-        <f t="shared" si="11"/>
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="AG5" s="14">
+        <f t="shared" si="16"/>
+        <v>500</v>
+      </c>
+      <c r="AH5" s="14">
+        <f t="shared" ref="AH5:AO5" si="17">kD_zandbaan</f>
+        <v>500</v>
+      </c>
+      <c r="AI5" s="14">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="AJ5" s="14">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="AK5" s="14">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="AL5" s="14">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="AM5" s="14">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="AN5" s="14">
+        <f t="shared" si="17"/>
+        <v>500</v>
+      </c>
+      <c r="AO5" s="14">
+        <f t="shared" si="17"/>
         <v>500</v>
       </c>
     </row>
     <row r="6" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A6" s="6" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
       <c r="B6" s="2">
         <v>0</v>
@@ -1919,7 +2154,7 @@
       <c r="J6" s="2">
         <v>0</v>
       </c>
-      <c r="K6" s="3">
+      <c r="K6" s="15">
         <v>0</v>
       </c>
       <c r="L6" s="3">
@@ -1961,7 +2196,7 @@
       <c r="X6" s="3">
         <v>0</v>
       </c>
-      <c r="Y6" s="3">
+      <c r="Y6" s="15">
         <v>0</v>
       </c>
       <c r="Z6" s="4">
@@ -1985,35 +2220,35 @@
       <c r="AF6" s="4">
         <v>0</v>
       </c>
-      <c r="AG6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AI6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AK6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AM6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AN6" s="17">
-        <v>0</v>
-      </c>
-      <c r="AO6" s="14"/>
+      <c r="AG6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AH6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AI6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AJ6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AK6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AL6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AN6" s="14">
+        <v>0</v>
+      </c>
+      <c r="AO6" s="11"/>
     </row>
     <row r="7" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A7" s="6" t="s">
-        <v>9</v>
+        <v>29</v>
       </c>
       <c r="B7" s="2">
         <v>500</v>
@@ -2042,50 +2277,50 @@
       <c r="J7" s="2">
         <v>500</v>
       </c>
-      <c r="K7" s="3">
-        <v>500</v>
+      <c r="K7" s="15">
+        <v>10</v>
       </c>
       <c r="L7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="M7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="N7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="O7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="P7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="Q7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="R7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="S7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="T7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="U7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="V7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="W7" s="3">
-        <v>500</v>
+        <v>10</v>
       </c>
       <c r="X7" s="3">
-        <v>500</v>
-      </c>
-      <c r="Y7" s="3">
-        <v>500</v>
+        <v>10</v>
+      </c>
+      <c r="Y7" s="15">
+        <v>10</v>
       </c>
       <c r="Z7" s="4">
         <v>500</v>
@@ -2108,37 +2343,37 @@
       <c r="AF7" s="4">
         <v>500</v>
       </c>
-      <c r="AG7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AH7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AI7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AJ7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AK7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AL7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AM7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AN7" s="17">
-        <v>500</v>
-      </c>
-      <c r="AO7" s="17">
+      <c r="AG7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AH7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AI7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AJ7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AK7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AL7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AM7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AN7" s="14">
+        <v>500</v>
+      </c>
+      <c r="AO7" s="14">
         <v>500</v>
       </c>
     </row>
     <row r="8" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A8" s="6" t="s">
-        <v>7</v>
+        <v>31</v>
       </c>
       <c r="B8" s="2">
         <v>2000</v>
@@ -2167,7 +2402,7 @@
       <c r="J8" s="2">
         <v>2000</v>
       </c>
-      <c r="K8" s="3">
+      <c r="K8" s="15">
         <v>2000</v>
       </c>
       <c r="L8" s="3">
@@ -2209,7 +2444,7 @@
       <c r="X8" s="3">
         <v>2000</v>
       </c>
-      <c r="Y8" s="3">
+      <c r="Y8" s="15">
         <v>2000</v>
       </c>
       <c r="Z8" s="4">
@@ -2233,37 +2468,37 @@
       <c r="AF8" s="4">
         <v>2000</v>
       </c>
-      <c r="AG8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AH8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AI8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AJ8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AK8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AL8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AM8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AN8" s="17">
-        <v>2000</v>
-      </c>
-      <c r="AO8" s="17">
+      <c r="AG8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AH8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AI8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AJ8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AK8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AL8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AM8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AN8" s="14">
+        <v>2000</v>
+      </c>
+      <c r="AO8" s="14">
         <v>2000</v>
       </c>
     </row>
     <row r="9" spans="1:41" x14ac:dyDescent="0.25">
       <c r="A9" s="6" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
       <c r="B9" s="2">
         <v>0</v>
@@ -2292,7 +2527,7 @@
       <c r="J9" s="2">
         <v>0</v>
       </c>
-      <c r="K9" s="3">
+      <c r="K9" s="15">
         <v>0</v>
       </c>
       <c r="L9" s="3">
@@ -2334,7 +2569,7 @@
       <c r="X9" s="3">
         <v>0</v>
       </c>
-      <c r="Y9" s="3">
+      <c r="Y9" s="15">
         <v>0</v>
       </c>
       <c r="Z9" s="4">
@@ -2358,159 +2593,205 @@
       <c r="AF9" s="4">
         <v>0</v>
       </c>
-      <c r="AG9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AH9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AI9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AJ9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AK9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AL9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AM9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AN9" s="17">
-        <v>0</v>
-      </c>
-      <c r="AO9" s="14"/>
+      <c r="AG9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AH9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AI9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AJ9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AK9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AL9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AM9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AN9" s="14">
+        <v>0</v>
+      </c>
+      <c r="AO9" s="11"/>
     </row>
     <row r="11" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A11" s="7" t="s">
-        <v>0</v>
+      <c r="B11" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="D11" s="6" t="s">
+        <v>3</v>
+      </c>
+      <c r="E11" s="6" t="s">
+        <v>1</v>
+      </c>
+      <c r="F11" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="G11" s="6" t="s">
+        <v>4</v>
+      </c>
+      <c r="H11" s="6" t="s">
+        <v>2</v>
+      </c>
+      <c r="I11" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="J11" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="K11" s="6" t="s">
+        <v>35</v>
       </c>
     </row>
     <row r="12" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A12" s="8" t="s">
-        <v>29</v>
-      </c>
+      <c r="A12" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="B12" s="16"/>
+      <c r="C12" s="16"/>
+      <c r="D12" s="16"/>
+      <c r="E12" s="16"/>
+      <c r="G12" s="16"/>
+      <c r="H12" s="16"/>
+      <c r="J12" s="16"/>
     </row>
     <row r="13" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A13" s="9" t="s">
-        <v>1</v>
+      <c r="A13" s="8" t="s">
+        <v>27</v>
       </c>
     </row>
     <row r="14" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A14" s="10" t="s">
-        <v>13</v>
-      </c>
+      <c r="A14" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="H14" s="16"/>
+      <c r="J14" s="16"/>
+      <c r="K14" s="16"/>
     </row>
     <row r="15" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A15" s="11" t="s">
-        <v>2</v>
-      </c>
+      <c r="A15" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B15" s="16"/>
+      <c r="C15" s="16"/>
+      <c r="D15" s="16"/>
+      <c r="E15" s="16"/>
+      <c r="G15" s="16"/>
+      <c r="H15" s="16"/>
+      <c r="J15" s="16"/>
     </row>
     <row r="16" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A16" s="12" t="s">
-        <v>3</v>
+      <c r="A16" s="14" t="s">
+        <v>32</v>
       </c>
     </row>
-    <row r="18" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>14</v>
+        <v>8</v>
       </c>
       <c r="B18" s="1">
         <v>0.5</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
       <c r="B19" s="1">
         <v>1</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>17</v>
+        <v>11</v>
       </c>
     </row>
-    <row r="20" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>27</v>
+        <v>21</v>
       </c>
       <c r="B20" s="1">
         <f>mv-draindiepte</f>
         <v>-0.5</v>
       </c>
     </row>
-    <row r="21" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>18</v>
+        <v>12</v>
       </c>
       <c r="B21" s="1" t="s">
-        <v>19</v>
+        <v>13</v>
       </c>
     </row>
-    <row r="22" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>20</v>
+        <v>14</v>
       </c>
       <c r="B22" s="1">
         <v>0.6</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>22</v>
+        <v>16</v>
       </c>
     </row>
-    <row r="23" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="B23" s="1">
         <f>draindiepte-GHG</f>
         <v>0.4</v>
       </c>
       <c r="C23" s="1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="24" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
         <v>17</v>
       </c>
+      <c r="B24" s="12">
+        <v>7.0000000000000001E-3</v>
+      </c>
+      <c r="C24" s="1" t="s">
+        <v>18</v>
+      </c>
     </row>
-    <row r="24" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>23</v>
-      </c>
-      <c r="B24" s="15">
-        <v>7.0000000000000001E-3</v>
-      </c>
-      <c r="C24" s="1" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="25" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
       <c r="B25" s="1">
         <f>opbolling/flux</f>
         <v>57.142857142857146</v>
       </c>
       <c r="C25" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="26" spans="1:41" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="27" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>26</v>
       </c>
+      <c r="B27" s="1">
+        <v>500</v>
+      </c>
+      <c r="D27" s="1" t="s">
+        <v>22</v>
+      </c>
     </row>
-    <row r="27" spans="1:41" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>34</v>
-      </c>
-      <c r="B27" s="1">
-        <v>500</v>
-      </c>
-      <c r="D27" s="1" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="29" spans="1:41" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:41" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="29" spans="1:41" hidden="1" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>1</v>
       </c>
@@ -2519,35 +2800,35 @@
         <v>2</v>
       </c>
       <c r="C29" s="1">
-        <f t="shared" ref="C29:AG29" si="12">B29+1</f>
+        <f t="shared" ref="C29:AG29" si="18">B29+1</f>
         <v>3</v>
       </c>
       <c r="D29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>4</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>5</v>
       </c>
       <c r="F29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>6</v>
       </c>
       <c r="G29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>7</v>
       </c>
       <c r="H29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>8</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>9</v>
       </c>
       <c r="J29" s="1">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>10</v>
       </c>
       <c r="K29" s="1" t="e">
@@ -2555,11 +2836,11 @@
         <v>#REF!</v>
       </c>
       <c r="L29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="M29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="N29" s="1" t="e">
@@ -2567,11 +2848,11 @@
         <v>#REF!</v>
       </c>
       <c r="O29" s="1" t="e">
-        <f t="shared" ref="O29" si="13">N29+1</f>
+        <f t="shared" ref="O29" si="19">N29+1</f>
         <v>#REF!</v>
       </c>
       <c r="P29" s="1" t="e">
-        <f t="shared" ref="P29" si="14">O29+1</f>
+        <f t="shared" ref="P29" si="20">O29+1</f>
         <v>#REF!</v>
       </c>
       <c r="Z29" s="1" t="e">
@@ -2579,31 +2860,31 @@
         <v>#REF!</v>
       </c>
       <c r="AA29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AB29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AC29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AD29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AE29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AF29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AG29" s="1" t="e">
-        <f t="shared" si="12"/>
+        <f t="shared" si="18"/>
         <v>#REF!</v>
       </c>
       <c r="AH29" s="1" t="e">
@@ -2611,35 +2892,35 @@
         <v>#REF!</v>
       </c>
       <c r="AI29" s="1" t="e">
-        <f t="shared" ref="AI29:AO29" si="15">AH29+1</f>
+        <f t="shared" ref="AI29:AO29" si="21">AH29+1</f>
         <v>#REF!</v>
       </c>
       <c r="AJ29" s="1" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
       <c r="AK29" s="1" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
       <c r="AL29" s="1" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
       <c r="AM29" s="1" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
       <c r="AN29" s="1" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
       <c r="AO29" s="1" t="e">
-        <f t="shared" si="15"/>
+        <f t="shared" si="21"/>
         <v>#REF!</v>
       </c>
     </row>
-    <row r="37" spans="13:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="13:14" hidden="1" x14ac:dyDescent="0.25">
       <c r="M37" s="1">
         <f>1600+3000</f>
         <v>4600</v>
@@ -2649,6 +2930,8 @@
         <v>6100</v>
       </c>
     </row>
+    <row r="38" spans="13:14" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="39" spans="13:14" hidden="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>